<commit_message>
comments and gitignore updates
</commit_message>
<xml_diff>
--- a/Paper/Draft 2 Comments.xlsx
+++ b/Paper/Draft 2 Comments.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meenu/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G7-DS\Documents\GitHub\SMU_Masters_PST\Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44170A38-18BC-DC4B-BC9E-6EC08B25CC15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8333224C-EFC8-4414-BB48-7869AB072466}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32520" windowHeight="17740" xr2:uid="{B81380B8-F88B-403B-AB49-A53BE6AEB6FD}"/>
+    <workbookView xWindow="-9276" yWindow="2604" windowWidth="17280" windowHeight="8964" xr2:uid="{B81380B8-F88B-403B-AB49-A53BE6AEB6FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$D$73</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="80">
   <si>
     <t>General Comments:</t>
   </si>
@@ -264,6 +267,9 @@
   </si>
   <si>
     <t xml:space="preserve">deferred </t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -307,7 +313,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -332,6 +338,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -345,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -364,6 +376,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,50 +698,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC108106-3399-4C3B-B692-EA06FB2A3CEF}">
   <dimension ref="A1:D143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="122.1640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="41.1640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="122.109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="41.109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C1" s="3"/>
       <c r="D1" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C2" s="1"/>
       <c r="D2" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C3" s="2"/>
       <c r="D3" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="95" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="104.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="38" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>3</v>
       </c>
@@ -736,238 +752,238 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="209" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="191.4" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="76" x14ac:dyDescent="0.2">
+      <c r="B10" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="87" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="38" x14ac:dyDescent="0.2">
+      <c r="B11" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="38" x14ac:dyDescent="0.2">
+      <c r="B12" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="38" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="57" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="76" x14ac:dyDescent="0.2">
+      <c r="B19" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="38" x14ac:dyDescent="0.2">
+      <c r="B20" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="38" x14ac:dyDescent="0.2">
+      <c r="B21" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="57" x14ac:dyDescent="0.2">
+      <c r="B23" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B24" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="38" x14ac:dyDescent="0.2">
+      <c r="B25" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B26" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="114" x14ac:dyDescent="0.2">
+      <c r="B26" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="104.4" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B27" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="57" x14ac:dyDescent="0.2">
+      <c r="B27" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="57" x14ac:dyDescent="0.2">
+      <c r="B28" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B29" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="76" x14ac:dyDescent="0.2">
+      <c r="B29" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="57" x14ac:dyDescent="0.2">
+      <c r="B30" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="38" x14ac:dyDescent="0.2">
+      <c r="B31" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="38" x14ac:dyDescent="0.2">
+      <c r="B32" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B34" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B34" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B35" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="57" x14ac:dyDescent="0.2">
+      <c r="B35" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B36" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B36" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B37" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="38" x14ac:dyDescent="0.2">
+      <c r="B37" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>33</v>
       </c>
@@ -975,7 +991,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="38" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>34</v>
       </c>
@@ -983,7 +999,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
         <v>35</v>
       </c>
@@ -991,7 +1007,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>36</v>
       </c>
@@ -999,7 +1015,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="57" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>37</v>
       </c>
@@ -1007,15 +1023,15 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B43" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B43" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>39</v>
       </c>
@@ -1023,15 +1039,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B45" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B45" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>41</v>
       </c>
@@ -1039,7 +1055,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
         <v>42</v>
       </c>
@@ -1047,36 +1063,36 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="38" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="76" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B50" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="38" x14ac:dyDescent="0.2">
+      <c r="B50" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B51" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="38" x14ac:dyDescent="0.2">
+      <c r="B51" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>47</v>
       </c>
@@ -1084,12 +1100,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="76" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>49</v>
       </c>
@@ -1097,7 +1113,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="38" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="s">
         <v>50</v>
       </c>
@@ -1105,7 +1121,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="s">
         <v>51</v>
       </c>
@@ -1113,7 +1129,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="38" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="s">
         <v>52</v>
       </c>
@@ -1121,12 +1137,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="s">
         <v>54</v>
       </c>
@@ -1134,7 +1150,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="s">
         <v>55</v>
       </c>
@@ -1142,7 +1158,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="38" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
         <v>56</v>
       </c>
@@ -1150,7 +1166,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="s">
         <v>57</v>
       </c>
@@ -1158,7 +1174,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="38" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
         <v>58</v>
       </c>
@@ -1166,12 +1182,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="57" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
         <v>60</v>
       </c>
@@ -1179,7 +1195,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
         <v>61</v>
       </c>
@@ -1187,7 +1203,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="38" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
         <v>62</v>
       </c>
@@ -1195,7 +1211,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A68" s="8" t="s">
         <v>63</v>
       </c>
@@ -1203,7 +1219,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="38" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="s">
         <v>64</v>
       </c>
@@ -1211,7 +1227,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
         <v>65</v>
       </c>
@@ -1219,12 +1235,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
         <v>67</v>
       </c>
@@ -1232,7 +1248,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
         <v>68</v>
       </c>
@@ -1240,217 +1256,218 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" s="9"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="9"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="9"/>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" s="9"/>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="9"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="9"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="9"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" s="9"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" s="9"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" s="9"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" s="9"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" s="9"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" s="9"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87" s="9"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" s="9"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" s="9"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" s="9"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" s="9"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" s="9"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" s="9"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" s="9"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" s="9"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" s="9"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" s="9"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" s="9"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" s="9"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" s="9"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A101" s="9"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A102" s="9"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A103" s="9"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A104" s="9"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A105" s="9"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A106" s="9"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A107" s="9"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108" s="9"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A109" s="9"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A110" s="9"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A111" s="9"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A112" s="9"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A113" s="9"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114" s="9"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A115" s="9"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A116" s="9"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A117" s="9"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A118" s="9"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A119" s="9"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A120" s="9"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A121" s="9"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A122" s="9"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A123" s="9"/>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A124" s="9"/>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A125" s="9"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A126" s="9"/>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A127" s="9"/>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A128" s="9"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A129" s="9"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A130" s="9"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A131" s="9"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A132" s="9"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A133" s="9"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A134" s="9"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A135" s="9"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A136" s="9"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A137" s="9"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A138" s="9"/>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A139" s="9"/>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A140" s="9"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A141" s="9"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A142" s="9"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A143" s="9"/>
     </row>
   </sheetData>
+  <autoFilter ref="A4:D73" xr:uid="{F1479100-812D-4207-A948-139AE247E2DF}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>